<commit_message>
Initial Player's turn value to 1 Documentation updated
</commit_message>
<xml_diff>
--- a/Documents/CShap_Project_TestCase.xlsx
+++ b/Documents/CShap_Project_TestCase.xlsx
@@ -292,6 +292,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -300,24 +318,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,15 +625,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="76.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="49.5703125" style="3" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
@@ -644,7 +644,7 @@
       <c r="A2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -665,13 +665,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -682,11 +682,11 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -697,13 +697,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="9">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -714,13 +714,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="9">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -731,13 +731,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="9">
         <v>5</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -748,11 +748,11 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="9">
         <v>6</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -763,11 +763,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="9">
         <v>7</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -778,13 +778,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="9">
         <v>8</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -795,11 +795,11 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="9">
         <v>9</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -810,13 +810,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="9">
         <v>10</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -827,11 +827,11 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="9">
         <v>11</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -842,11 +842,11 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="A16" s="9">
         <v>12</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -857,13 +857,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="A17" s="9">
         <v>13</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -874,11 +874,11 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="A18" s="9">
         <v>14</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="14" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -889,13 +889,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="A19" s="9">
         <v>15</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -906,11 +906,11 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+      <c r="A20" s="9">
         <v>16</v>
       </c>
       <c r="B20" s="12"/>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -921,11 +921,11 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="A21" s="9">
         <v>17</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -936,11 +936,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
+      <c r="A22" s="9">
         <v>18</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="14" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="4" t="s">

</xml_diff>